<commit_message>
tambahkan murojaah kamis dan jumat
</commit_message>
<xml_diff>
--- a/buku-tahfidz-lengkap/murojaah.xlsx
+++ b/buku-tahfidz-lengkap/murojaah.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E707ED5-E985-4A5C-82D2-19D972E9D3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5C1598-DEAD-41DB-AE5E-7538277D5A91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="السبت" sheetId="1" r:id="rId1"/>
-    <sheet name="بعد العشاء" sheetId="2" r:id="rId2"/>
+    <sheet name="الخميس" sheetId="4" r:id="rId1"/>
+    <sheet name="الجمعة" sheetId="3" r:id="rId2"/>
+    <sheet name="السبت" sheetId="1" r:id="rId3"/>
+    <sheet name="بعد العشاء" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">السبت!$A$1:$G$51</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'بعد العشاء'!$A$1:$U$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">الجمعة!$A$1:$G$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">الخميس!$A$1:$G$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">السبت!$A$1:$G$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'بعد العشاء'!$A$1:$U$46</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="17">
   <si>
     <t>شهر:</t>
   </si>
@@ -70,6 +74,12 @@
   </si>
   <si>
     <t>في قسم التوقيع، إذا أكمل الطلاب المراجعة يوم الأحد، يُملأ بـ (T)</t>
+  </si>
+  <si>
+    <t>المراجعة يوم الخميس</t>
+  </si>
+  <si>
+    <t>المراجعة يوم الجمعة</t>
   </si>
 </sst>
 </file>
@@ -324,9 +334,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -340,6 +347,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -624,6 +634,1222 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE98E9D9-A830-40BD-8B1E-FDF0D3757CDC}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="F2" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="F10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="19"/>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="5">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="F18" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="5">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5">
+        <v>2</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="F26" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="19"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="5">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5">
+        <v>4</v>
+      </c>
+      <c r="D27" s="5">
+        <v>3</v>
+      </c>
+      <c r="E27" s="5">
+        <v>2</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="F34" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="5">
+        <v>5</v>
+      </c>
+      <c r="C35" s="5">
+        <v>4</v>
+      </c>
+      <c r="D35" s="5">
+        <v>3</v>
+      </c>
+      <c r="E35" s="5">
+        <v>2</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="F42" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="19"/>
+    </row>
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="5">
+        <v>5</v>
+      </c>
+      <c r="C43" s="5">
+        <v>4</v>
+      </c>
+      <c r="D43" s="5">
+        <v>3</v>
+      </c>
+      <c r="E43" s="5">
+        <v>2</v>
+      </c>
+      <c r="F43" s="5">
+        <v>1</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="F18:G18"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
+  <pageSetup paperSize="11" scale="75" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B35654-7D4C-40FB-9CB0-54DF889303FB}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="F2" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="F10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="19"/>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="5">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="F18" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="5">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5">
+        <v>2</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="F26" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="19"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="5">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5">
+        <v>4</v>
+      </c>
+      <c r="D27" s="5">
+        <v>3</v>
+      </c>
+      <c r="E27" s="5">
+        <v>2</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="F34" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="5">
+        <v>5</v>
+      </c>
+      <c r="C35" s="5">
+        <v>4</v>
+      </c>
+      <c r="D35" s="5">
+        <v>3</v>
+      </c>
+      <c r="E35" s="5">
+        <v>2</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="F42" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="19"/>
+    </row>
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="5">
+        <v>5</v>
+      </c>
+      <c r="C43" s="5">
+        <v>4</v>
+      </c>
+      <c r="D43" s="5">
+        <v>3</v>
+      </c>
+      <c r="E43" s="5">
+        <v>2</v>
+      </c>
+      <c r="F43" s="5">
+        <v>1</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="F18:G18"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
+  <pageSetup paperSize="11" scale="75" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1231,14 +2457,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882DB66F-B835-415A-A586-21D736E9E3C6}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
@@ -1249,37 +2475,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
+      <c r="A1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
     </row>
     <row r="2" spans="1:21" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
-      <c r="D2" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="23"/>
+      <c r="D2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="22"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -1293,42 +2519,42 @@
       <c r="P2" s="18"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
-      <c r="T2" s="23" t="s">
+      <c r="T2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="U2" s="23"/>
+      <c r="U2" s="22"/>
     </row>
     <row r="3" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21" t="s">
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
       <c r="U3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1354,7 +2580,7 @@
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
       <c r="T4" s="12"/>
-      <c r="U4" s="24">
+      <c r="U4" s="23">
         <v>1</v>
       </c>
     </row>
@@ -1379,7 +2605,7 @@
       <c r="R5" s="14"/>
       <c r="S5" s="14"/>
       <c r="T5" s="15"/>
-      <c r="U5" s="25"/>
+      <c r="U5" s="24"/>
     </row>
     <row r="6" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
@@ -1402,7 +2628,7 @@
       <c r="R6" s="14"/>
       <c r="S6" s="14"/>
       <c r="T6" s="15"/>
-      <c r="U6" s="25"/>
+      <c r="U6" s="24"/>
     </row>
     <row r="7" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
@@ -1425,7 +2651,7 @@
       <c r="R7" s="17"/>
       <c r="S7" s="17"/>
       <c r="T7" s="10"/>
-      <c r="U7" s="26"/>
+      <c r="U7" s="25"/>
     </row>
     <row r="8" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
@@ -1448,7 +2674,7 @@
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
       <c r="T8" s="12"/>
-      <c r="U8" s="24">
+      <c r="U8" s="23">
         <v>2</v>
       </c>
     </row>
@@ -1473,7 +2699,7 @@
       <c r="R9" s="14"/>
       <c r="S9" s="14"/>
       <c r="T9" s="15"/>
-      <c r="U9" s="25"/>
+      <c r="U9" s="24"/>
     </row>
     <row r="10" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
@@ -1496,7 +2722,7 @@
       <c r="R10" s="14"/>
       <c r="S10" s="14"/>
       <c r="T10" s="15"/>
-      <c r="U10" s="25"/>
+      <c r="U10" s="24"/>
     </row>
     <row r="11" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
@@ -1519,7 +2745,7 @@
       <c r="R11" s="17"/>
       <c r="S11" s="17"/>
       <c r="T11" s="10"/>
-      <c r="U11" s="26"/>
+      <c r="U11" s="25"/>
     </row>
     <row r="12" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
@@ -1542,7 +2768,7 @@
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
       <c r="T12" s="12"/>
-      <c r="U12" s="24">
+      <c r="U12" s="23">
         <v>3</v>
       </c>
     </row>
@@ -1567,7 +2793,7 @@
       <c r="R13" s="14"/>
       <c r="S13" s="14"/>
       <c r="T13" s="15"/>
-      <c r="U13" s="25"/>
+      <c r="U13" s="24"/>
     </row>
     <row r="14" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
@@ -1590,7 +2816,7 @@
       <c r="R14" s="14"/>
       <c r="S14" s="14"/>
       <c r="T14" s="15"/>
-      <c r="U14" s="25"/>
+      <c r="U14" s="24"/>
     </row>
     <row r="15" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
@@ -1613,7 +2839,7 @@
       <c r="R15" s="17"/>
       <c r="S15" s="17"/>
       <c r="T15" s="10"/>
-      <c r="U15" s="26"/>
+      <c r="U15" s="25"/>
     </row>
     <row r="16" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
@@ -1636,7 +2862,7 @@
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
       <c r="T16" s="12"/>
-      <c r="U16" s="24">
+      <c r="U16" s="23">
         <v>4</v>
       </c>
     </row>
@@ -1661,7 +2887,7 @@
       <c r="R17" s="14"/>
       <c r="S17" s="14"/>
       <c r="T17" s="15"/>
-      <c r="U17" s="25"/>
+      <c r="U17" s="24"/>
     </row>
     <row r="18" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
@@ -1684,7 +2910,7 @@
       <c r="R18" s="14"/>
       <c r="S18" s="14"/>
       <c r="T18" s="15"/>
-      <c r="U18" s="25"/>
+      <c r="U18" s="24"/>
     </row>
     <row r="19" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
@@ -1707,7 +2933,7 @@
       <c r="R19" s="17"/>
       <c r="S19" s="17"/>
       <c r="T19" s="10"/>
-      <c r="U19" s="26"/>
+      <c r="U19" s="25"/>
     </row>
     <row r="20" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
@@ -1730,7 +2956,7 @@
       <c r="R20" s="11"/>
       <c r="S20" s="11"/>
       <c r="T20" s="12"/>
-      <c r="U20" s="24">
+      <c r="U20" s="23">
         <v>5</v>
       </c>
     </row>
@@ -1755,7 +2981,7 @@
       <c r="R21" s="14"/>
       <c r="S21" s="14"/>
       <c r="T21" s="15"/>
-      <c r="U21" s="25"/>
+      <c r="U21" s="24"/>
     </row>
     <row r="22" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
@@ -1778,7 +3004,7 @@
       <c r="R22" s="14"/>
       <c r="S22" s="14"/>
       <c r="T22" s="15"/>
-      <c r="U22" s="25"/>
+      <c r="U22" s="24"/>
     </row>
     <row r="23" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
@@ -1801,16 +3027,16 @@
       <c r="R23" s="17"/>
       <c r="S23" s="17"/>
       <c r="T23" s="10"/>
-      <c r="U23" s="26"/>
+      <c r="U23" s="25"/>
     </row>
     <row r="24" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:21" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
-      <c r="D25" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="23"/>
+      <c r="D25" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="22"/>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
@@ -1824,42 +3050,42 @@
       <c r="P25" s="18"/>
       <c r="Q25" s="18"/>
       <c r="R25" s="18"/>
-      <c r="T25" s="23" t="s">
+      <c r="T25" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="U25" s="23"/>
+      <c r="U25" s="22"/>
     </row>
     <row r="26" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21" t="s">
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21" t="s">
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="R26" s="21"/>
-      <c r="S26" s="21"/>
-      <c r="T26" s="21"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
       <c r="U26" s="8" t="s">
         <v>3</v>
       </c>
@@ -1933,7 +3159,7 @@
       <c r="R29" s="14"/>
       <c r="S29" s="14"/>
       <c r="T29" s="15"/>
-      <c r="U29" s="21"/>
+      <c r="U29" s="26"/>
     </row>
     <row r="30" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16"/>
@@ -1956,7 +3182,7 @@
       <c r="R30" s="17"/>
       <c r="S30" s="17"/>
       <c r="T30" s="10"/>
-      <c r="U30" s="21"/>
+      <c r="U30" s="26"/>
     </row>
     <row r="31" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
@@ -2027,7 +3253,7 @@
       <c r="R33" s="14"/>
       <c r="S33" s="14"/>
       <c r="T33" s="15"/>
-      <c r="U33" s="21"/>
+      <c r="U33" s="26"/>
     </row>
     <row r="34" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
@@ -2050,7 +3276,7 @@
       <c r="R34" s="17"/>
       <c r="S34" s="17"/>
       <c r="T34" s="10"/>
-      <c r="U34" s="21"/>
+      <c r="U34" s="26"/>
     </row>
     <row r="35" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
@@ -2121,7 +3347,7 @@
       <c r="R37" s="14"/>
       <c r="S37" s="14"/>
       <c r="T37" s="15"/>
-      <c r="U37" s="21"/>
+      <c r="U37" s="26"/>
     </row>
     <row r="38" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
@@ -2144,7 +3370,7 @@
       <c r="R38" s="17"/>
       <c r="S38" s="17"/>
       <c r="T38" s="10"/>
-      <c r="U38" s="21"/>
+      <c r="U38" s="26"/>
     </row>
     <row r="39" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
@@ -2215,7 +3441,7 @@
       <c r="R41" s="14"/>
       <c r="S41" s="14"/>
       <c r="T41" s="15"/>
-      <c r="U41" s="21"/>
+      <c r="U41" s="26"/>
     </row>
     <row r="42" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
@@ -2238,7 +3464,7 @@
       <c r="R42" s="17"/>
       <c r="S42" s="17"/>
       <c r="T42" s="10"/>
-      <c r="U42" s="21"/>
+      <c r="U42" s="26"/>
     </row>
     <row r="43" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
@@ -2309,7 +3535,7 @@
       <c r="R45" s="14"/>
       <c r="S45" s="14"/>
       <c r="T45" s="15"/>
-      <c r="U45" s="21"/>
+      <c r="U45" s="26"/>
     </row>
     <row r="46" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
@@ -2332,10 +3558,20 @@
       <c r="R46" s="17"/>
       <c r="S46" s="17"/>
       <c r="T46" s="10"/>
-      <c r="U46" s="21"/>
+      <c r="U46" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="U27:U30"/>
+    <mergeCell ref="U31:U34"/>
+    <mergeCell ref="U35:U38"/>
+    <mergeCell ref="U39:U42"/>
+    <mergeCell ref="U43:U46"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="I26:L26"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="Q26:T26"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="T25:U25"/>
@@ -2351,16 +3587,6 @@
     <mergeCell ref="Q3:T3"/>
     <mergeCell ref="U4:U7"/>
     <mergeCell ref="M3:P3"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="I26:L26"/>
-    <mergeCell ref="M26:P26"/>
-    <mergeCell ref="Q26:T26"/>
-    <mergeCell ref="U27:U30"/>
-    <mergeCell ref="U31:U34"/>
-    <mergeCell ref="U35:U38"/>
-    <mergeCell ref="U39:U42"/>
-    <mergeCell ref="U43:U46"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>

</xml_diff>